<commit_message>
Create script to load MSA data
</commit_message>
<xml_diff>
--- a/NyAl_GVB_PM10_MSA_2010-21_LN.xlsx
+++ b/NyAl_GVB_PM10_MSA_2010-21_LN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lovisa\Documents\GitHub\Tjaernoe2022-group3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E0FE3B-FE6F-487C-B046-3A7127747FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94273720-0E3B-4D2B-8825-880257F12C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -58,13 +58,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="170" formatCode="0.0"/>
-    <numFmt numFmtId="171" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy"/>
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -141,33 +141,33 @@
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -391,7 +391,7 @@
   <dimension ref="A1:D1913"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>